<commit_message>
revise and well down
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -3,14 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3580" yWindow="500" windowWidth="21820" windowHeight="13900" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14400" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="查看销售金额2022.11-2023.1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'查看销售金额2022.11-2023.1'!$A$1:$CI$193</definedName>
-  </definedNames>
+  <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -824,16 +822,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:CI200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AO1" sqref="AO1"/>
-      <selection pane="bottomLeft" activeCell="AV198" sqref="AV198"/>
+      <selection pane="bottomLeft" activeCell="X147" sqref="X147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" outlineLevelRow="1"/>
@@ -853,6 +851,9 @@
     <col hidden="1" width="13" customWidth="1" style="46" min="27" max="43"/>
     <col hidden="1" width="13" customWidth="1" style="46" min="47" max="60"/>
     <col hidden="1" width="13" customWidth="1" style="46" min="71" max="77"/>
+    <col width="8.83203125" customWidth="1" style="46" min="78" max="88"/>
+    <col width="8.83203125" customWidth="1" style="27" min="89" max="89"/>
+    <col width="8.83203125" customWidth="1" style="27" min="90" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" outlineLevel="1" ht="42.5" customFormat="1" customHeight="1" s="18">
@@ -22801,13 +22802,13 @@
         <v>0.828</v>
       </c>
       <c r="AR66" s="49" t="n">
-        <v>0.504</v>
+        <v>0.252</v>
       </c>
       <c r="AS66" s="49" t="n">
-        <v>0.828</v>
+        <v>0.9</v>
       </c>
       <c r="AT66" s="49" t="n">
-        <v>0.324</v>
+        <v>0.432</v>
       </c>
       <c r="AU66" s="24" t="n">
         <v>0</v>
@@ -23133,13 +23134,13 @@
         <v>0.4032</v>
       </c>
       <c r="AR67" s="49" t="n">
-        <v>0.2352</v>
+        <v>0.4368</v>
       </c>
       <c r="AS67" s="49" t="n">
-        <v>0.3696</v>
+        <v>0.6048</v>
       </c>
       <c r="AT67" s="49" t="n">
-        <v>0.2016</v>
+        <v>0.1008</v>
       </c>
       <c r="AU67" s="24" t="n">
         <v>0</v>
@@ -35159,13 +35160,13 @@
         <v>1.652</v>
       </c>
       <c r="AR104" s="49" t="n">
-        <v>0.28</v>
+        <v>0.364</v>
       </c>
       <c r="AS104" s="49" t="n">
         <v>1.904</v>
       </c>
       <c r="AT104" s="49" t="n">
-        <v>1.288</v>
+        <v>1.232</v>
       </c>
       <c r="AU104" s="24" t="n">
         <v>6.34</v>
@@ -36787,13 +36788,13 @@
         <v>8</v>
       </c>
       <c r="AR109" s="49" t="n">
-        <v>8.208</v>
+        <v>8.304</v>
       </c>
       <c r="AS109" s="49" t="n">
-        <v>14.724</v>
+        <v>14.964</v>
       </c>
       <c r="AT109" s="49" t="n">
-        <v>11.292</v>
+        <v>11.196</v>
       </c>
       <c r="AU109" s="24" t="n">
         <v>8.44</v>
@@ -41947,7 +41948,7 @@
         <v>0</v>
       </c>
       <c r="AR125" s="49" t="n">
-        <v>2.0832</v>
+        <v>1.2432</v>
       </c>
       <c r="AS125" s="49" t="n">
         <v>0</v>
@@ -42270,10 +42271,10 @@
         <v>0</v>
       </c>
       <c r="AS126" s="49" t="n">
-        <v>3.0576</v>
+        <v>3.1248</v>
       </c>
       <c r="AT126" s="49" t="n">
-        <v>1.6464</v>
+        <v>1.5792</v>
       </c>
       <c r="AU126" s="24" t="n">
         <v>0</v>
@@ -48367,13 +48368,13 @@
         <v>8.064</v>
       </c>
       <c r="AR145" s="49" t="n">
-        <v>5.236</v>
+        <v>4.956</v>
       </c>
       <c r="AS145" s="49" t="n">
-        <v>10.64</v>
+        <v>10.248</v>
       </c>
       <c r="AT145" s="49" t="n">
-        <v>5.18</v>
+        <v>5.124000000000001</v>
       </c>
       <c r="AU145" s="24" t="n">
         <v>0</v>
@@ -48836,173 +48837,173 @@
         <v/>
       </c>
     </row>
-    <row r="147" outlineLevel="1" s="46">
-      <c r="A147" s="24" t="n">
+    <row r="147" outlineLevel="1" customFormat="1" s="43">
+      <c r="A147" s="41" t="n">
         <v>142</v>
       </c>
-      <c r="B147" s="24" t="inlineStr">
+      <c r="B147" s="41" t="inlineStr">
         <is>
           <t>出口/Export</t>
         </is>
       </c>
-      <c r="C147" s="24" t="inlineStr">
+      <c r="C147" s="41" t="inlineStr">
         <is>
           <t>SHI</t>
         </is>
       </c>
-      <c r="D147" s="24" t="inlineStr">
+      <c r="D147" s="41" t="inlineStr">
         <is>
           <t>客户发展部</t>
         </is>
       </c>
-      <c r="E147" s="24" t="inlineStr">
+      <c r="E147" s="41" t="inlineStr">
         <is>
           <t>HC18所</t>
         </is>
       </c>
-      <c r="F147" s="24" t="inlineStr">
+      <c r="F147" s="41" t="inlineStr">
         <is>
           <t>廖剑涛/Kirk Kralapp/Joana</t>
         </is>
       </c>
-      <c r="G147" s="24" t="inlineStr">
+      <c r="G147" s="41" t="inlineStr">
         <is>
           <t>TLA100</t>
         </is>
       </c>
-      <c r="H147" s="24" t="inlineStr">
+      <c r="H147" s="41" t="inlineStr">
         <is>
           <t>TESLA, Inc</t>
         </is>
       </c>
-      <c r="I147" s="24" t="inlineStr">
+      <c r="I147" s="41" t="inlineStr">
         <is>
           <t>HC18</t>
         </is>
       </c>
-      <c r="J147" s="24" t="inlineStr">
+      <c r="J147" s="41" t="inlineStr">
         <is>
           <t>美洲</t>
         </is>
       </c>
-      <c r="K147" s="24" t="inlineStr">
+      <c r="K147" s="41" t="inlineStr">
         <is>
           <t>HC18</t>
         </is>
       </c>
-      <c r="L147" s="24" t="inlineStr">
+      <c r="L147" s="41" t="inlineStr">
         <is>
           <t>OEM</t>
         </is>
       </c>
-      <c r="M147" s="24" t="inlineStr">
+      <c r="M147" s="41" t="inlineStr">
         <is>
           <t>批量/SOP</t>
         </is>
       </c>
-      <c r="N147" s="24" t="inlineStr">
+      <c r="N147" s="41" t="inlineStr">
         <is>
           <t>集成模块/Integrated Module</t>
         </is>
       </c>
-      <c r="O147" s="24" t="inlineStr">
+      <c r="O147" s="41" t="inlineStr">
         <is>
           <t>新能源产品</t>
         </is>
       </c>
-      <c r="P147" s="24" t="inlineStr">
+      <c r="P147" s="41" t="inlineStr">
         <is>
           <t>事业五部</t>
         </is>
       </c>
-      <c r="Q147" s="24" t="inlineStr">
+      <c r="Q147" s="41" t="inlineStr">
         <is>
           <t>绍兴工厂</t>
         </is>
       </c>
-      <c r="R147" s="24" t="inlineStr">
+      <c r="R147" s="41" t="inlineStr">
         <is>
           <t>S/C/1739701-00-B/#/#</t>
         </is>
       </c>
-      <c r="S147" s="24" t="inlineStr">
+      <c r="S147" s="41" t="inlineStr">
         <is>
           <t>01320100090</t>
         </is>
       </c>
-      <c r="T147" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="U147" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="V147" s="24" t="inlineStr">
+      <c r="T147" s="41" t="n">
+        <v>0</v>
+      </c>
+      <c r="U147" s="41" t="n">
+        <v>0</v>
+      </c>
+      <c r="V147" s="41" t="inlineStr">
         <is>
           <t>ASY,RAPTOR,TC,MP2XL</t>
         </is>
       </c>
-      <c r="W147" s="24" t="n">
+      <c r="W147" s="41" t="n">
         <v>0</v>
       </c>
       <c r="X147" s="51" t="inlineStr">
         <is>
-          <t>1739701-00-B</t>
-        </is>
-      </c>
-      <c r="Y147" s="24" t="inlineStr">
+          <t>1739701-50-B</t>
+        </is>
+      </c>
+      <c r="Y147" s="41" t="inlineStr">
         <is>
           <t>批量SOP</t>
         </is>
       </c>
-      <c r="Z147" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA147" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB147" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC147" s="24" t="inlineStr">
+      <c r="Z147" s="41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA147" s="41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB147" s="41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC147" s="41" t="inlineStr">
         <is>
           <t>HC18（储能）</t>
         </is>
       </c>
-      <c r="AD147" s="24" t="inlineStr">
+      <c r="AD147" s="41" t="inlineStr">
         <is>
           <t>Raptor</t>
         </is>
       </c>
-      <c r="AE147" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF147" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG147" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH147" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI147" s="24" t="inlineStr">
+      <c r="AE147" s="41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF147" s="41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG147" s="41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH147" s="41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI147" s="41" t="inlineStr">
         <is>
           <t>美元/USD</t>
         </is>
       </c>
-      <c r="AJ147" s="24" t="n">
+      <c r="AJ147" s="41" t="n">
         <v>6.8</v>
       </c>
-      <c r="AK147" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL147" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM147" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN147" s="24" t="n">
+      <c r="AK147" s="41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL147" s="41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM147" s="41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN147" s="41" t="n">
         <v>0</v>
       </c>
       <c r="AO147" s="41" t="n">
@@ -49023,143 +49024,143 @@
       <c r="AT147" s="49" t="n">
         <v>0.0392</v>
       </c>
-      <c r="AU147" s="24" t="n">
+      <c r="AU147" s="41" t="n">
         <v>0.028</v>
       </c>
-      <c r="AV147" s="24" t="n">
+      <c r="AV147" s="41" t="n">
         <v>0.032</v>
       </c>
-      <c r="AW147" s="24" t="n">
+      <c r="AW147" s="41" t="n">
         <v>0.032</v>
       </c>
-      <c r="AX147" s="24" t="n">
+      <c r="AX147" s="41" t="n">
         <v>0.032</v>
       </c>
-      <c r="AY147" s="24" t="n">
+      <c r="AY147" s="41" t="n">
         <v>0.036</v>
       </c>
-      <c r="AZ147" s="24" t="n">
+      <c r="AZ147" s="41" t="n">
         <v>0.036</v>
       </c>
-      <c r="BA147" s="24" t="n">
+      <c r="BA147" s="41" t="n">
         <v>0.036</v>
       </c>
-      <c r="BB147" s="24" t="n">
+      <c r="BB147" s="41" t="n">
         <v>1250</v>
       </c>
-      <c r="BC147" s="24" t="n">
+      <c r="BC147" s="41" t="n">
         <v>1250</v>
       </c>
-      <c r="BD147" s="24" t="n">
+      <c r="BD147" s="41" t="n">
         <v>1250</v>
       </c>
-      <c r="BE147" s="24" t="n">
+      <c r="BE147" s="41" t="n">
         <v>1250</v>
       </c>
-      <c r="BF147" s="24" t="n">
+      <c r="BF147" s="41" t="n">
         <v>1250</v>
       </c>
-      <c r="BG147" s="24" t="n">
+      <c r="BG147" s="41" t="n">
         <v>1250</v>
       </c>
-      <c r="BH147" s="24" t="n">
+      <c r="BH147" s="41" t="n">
         <v>1250</v>
       </c>
-      <c r="BI147" s="24" t="n">
+      <c r="BI147" s="41" t="n">
         <v>1250</v>
       </c>
-      <c r="BJ147" s="24" t="n">
+      <c r="BJ147" s="41" t="n">
         <v>1250</v>
       </c>
-      <c r="BK147" s="24" t="n">
+      <c r="BK147" s="41" t="n">
         <v>1250</v>
       </c>
-      <c r="BL147" s="24" t="n">
+      <c r="BL147" s="41" t="n">
         <v>1250</v>
       </c>
-      <c r="BM147" s="24" t="n">
+      <c r="BM147" s="41" t="n">
         <v>1250</v>
       </c>
-      <c r="BN147" s="24" t="n">
+      <c r="BN147" s="41" t="n">
         <v>1250</v>
       </c>
-      <c r="BO147" s="24" t="n">
+      <c r="BO147" s="41" t="n">
         <v>1250</v>
       </c>
-      <c r="BP147" s="24" t="n">
+      <c r="BP147" s="41" t="n">
         <v>1250</v>
       </c>
-      <c r="BQ147" s="24" t="n">
+      <c r="BQ147" s="41" t="n">
         <v>1250</v>
       </c>
-      <c r="BR147" s="24" t="n">
+      <c r="BR147" s="41" t="n">
         <v>1250</v>
       </c>
-      <c r="BS147" s="24">
+      <c r="BS147" s="41">
         <f>BB147*AK147*$AJ147</f>
         <v/>
       </c>
-      <c r="BT147" s="24">
+      <c r="BT147" s="41">
         <f>BC147*AL147*$AJ147</f>
         <v/>
       </c>
-      <c r="BU147" s="24">
+      <c r="BU147" s="41">
         <f>BD147*AM147*$AJ147</f>
         <v/>
       </c>
-      <c r="BV147" s="26">
+      <c r="BV147" s="41">
         <f>BE147*AN147*$AJ147</f>
         <v/>
       </c>
-      <c r="BW147" s="26">
+      <c r="BW147" s="41">
         <f>BF147*AO147*$AJ147</f>
         <v/>
       </c>
-      <c r="BX147" s="26">
+      <c r="BX147" s="41">
         <f>AP147*BG147*$AJ147</f>
         <v/>
       </c>
-      <c r="BY147" s="24">
+      <c r="BY147" s="41">
         <f>AQ147*BH147*$AJ147</f>
         <v/>
       </c>
-      <c r="BZ147" s="24">
+      <c r="BZ147" s="41">
         <f>AR147*BI147*$AJ147</f>
         <v/>
       </c>
-      <c r="CA147" s="24">
+      <c r="CA147" s="41">
         <f>AS147*BJ147*$AJ147</f>
         <v/>
       </c>
-      <c r="CB147" s="24">
+      <c r="CB147" s="41">
         <f>AT147*BK147*$AJ147</f>
         <v/>
       </c>
-      <c r="CC147" s="24">
+      <c r="CC147" s="41">
         <f>AU147*BL147*$AJ147</f>
         <v/>
       </c>
-      <c r="CD147" s="24">
+      <c r="CD147" s="41">
         <f>AV147*BM147*$AJ147</f>
         <v/>
       </c>
-      <c r="CE147" s="24">
+      <c r="CE147" s="41">
         <f>AW147*BN147*$AJ147</f>
         <v/>
       </c>
-      <c r="CF147" s="24">
+      <c r="CF147" s="41">
         <f>AX147*BO147*$AJ147</f>
         <v/>
       </c>
-      <c r="CG147" s="24">
+      <c r="CG147" s="41">
         <f>AY147*BP147*$AJ147</f>
         <v/>
       </c>
-      <c r="CH147" s="24">
+      <c r="CH147" s="41">
         <f>AZ147*BQ147*$AJ147</f>
         <v/>
       </c>
-      <c r="CI147" s="24">
+      <c r="CI147" s="41">
         <f>BA147*BR147*$AJ147</f>
         <v/>
       </c>
@@ -65068,13 +65069,6 @@
     <row r="999" hidden="1" outlineLevel="1" s="46"/>
     <row r="1000" hidden="1" outlineLevel="1" s="46"/>
   </sheetData>
-  <autoFilter ref="A1:CI193">
-    <filterColumn colId="8">
-      <filters>
-        <filter val="宁波拓普集团股份有限公司"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <conditionalFormatting sqref="S1">
     <cfRule type="duplicateValues" priority="29" dxfId="0"/>
   </conditionalFormatting>

</xml_diff>